<commit_message>
so salvar planilhas atualizadas
</commit_message>
<xml_diff>
--- a/planilhaderotascc15.xlsx
+++ b/planilhaderotascc15.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Lucas\Desktop\Robo-Baixa-Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CE85909E-1B65-4376-9AC7-C4F344913187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{088669F2-926A-4558-B0FD-B6543C916D66}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CE85909E-1B65-4376-9AC7-C4F344913187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{391252FB-1C81-4CC0-90DE-8A98542016C0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="CC15" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -2978,24 +2978,24 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="3" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="3" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3379,8 +3379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1084"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A640" workbookViewId="0">
-      <selection activeCell="A372" sqref="A372:O1084"/>
+    <sheetView tabSelected="1" topLeftCell="A1063" workbookViewId="0">
+      <selection activeCell="D915" sqref="D915"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>